<commit_message>
Fixed an issue where a pronoum was wrong on the 1st Paragraph
</commit_message>
<xml_diff>
--- a/Templates/StudentProfile.xlsx
+++ b/Templates/StudentProfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clfilho/Dropbox (Personal)/Rec-Auto/Python Script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD75FA87-E99B-2745-8583-17A07C52F8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9F8923-C82A-7F4F-B6E2-BFCBDC85C536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37080" yWindow="460" windowWidth="33600" windowHeight="20500" xr2:uid="{8A1CF855-2C5B-F149-936A-A90AA29A5A87}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="117">
   <si>
     <t>First Name:</t>
   </si>
@@ -452,19 +452,22 @@
     <t>enjoys applying logical reasoning to solve problems, is very data driven and adepts at recognizing patterns</t>
   </si>
   <si>
-    <t>he</t>
-  </si>
-  <si>
     <t>Junior</t>
   </si>
   <si>
-    <t>Abeer</t>
-  </si>
-  <si>
-    <t>Bajpai</t>
-  </si>
-  <si>
     <t>MIT</t>
+  </si>
+  <si>
+    <t>&lt;- Add a Space here if no instituiton is required</t>
+  </si>
+  <si>
+    <t>she</t>
+  </si>
+  <si>
+    <t>Onebeer</t>
+  </si>
+  <si>
+    <t>Moreplease</t>
   </si>
 </sst>
 </file>
@@ -899,14 +902,14 @@
   <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="42.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="52.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="40.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.5" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.33203125" style="2" customWidth="1"/>
@@ -933,7 +936,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -941,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -950,7 +953,7 @@
         <v>58</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -986,7 +989,7 @@
         <v>66</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" s="4"/>
     </row>
@@ -995,9 +998,11 @@
         <v>71</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="4"/>
+        <v>112</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">

</xml_diff>